<commit_message>
Searching and filtering have been updated
</commit_message>
<xml_diff>
--- a/Cats-Cafe-Accounting-System/bin/Debug/net8.0-windows/.xlsx
+++ b/Cats-Cafe-Accounting-System/bin/Debug/net8.0-windows/.xlsx
@@ -92,8 +92,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D27" totalsRowShown="0">
-  <x:autoFilter ref="A1:D27"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0">
+  <x:autoFilter ref="A1:D22"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="isSelected"/>
     <x:tableColumn id="2" name="item"/>
@@ -392,7 +392,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D27"/>
+  <x:dimension ref="A1:D22"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -703,76 +703,6 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:4">
-      <x:c r="A23" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D23" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:4">
-      <x:c r="A24" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C24" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:4">
-      <x:c r="A25" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C25" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:4">
-      <x:c r="A26" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B26" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C26" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:4">
-      <x:c r="A27" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>

</xml_diff>